<commit_message>
errors de canvi de dni
</commit_message>
<xml_diff>
--- a/Gsport/Gsport/FitxersImport/Entrenadors.xlsx
+++ b/Gsport/Gsport/FitxersImport/Entrenadors.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>nom</t>
   </si>
@@ -98,6 +98,15 @@
   </si>
   <si>
     <t>Pedros</t>
+  </si>
+  <si>
+    <t>45625454i</t>
+  </si>
+  <si>
+    <t>Arnau</t>
+  </si>
+  <si>
+    <t>Taberner</t>
   </si>
 </sst>
 </file>
@@ -105,7 +114,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="d\-m\-yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="d\-m\-yyyy;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -169,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -191,16 +200,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -508,7 +523,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -544,7 +559,7 @@
         <v>20</v>
       </c>
       <c r="D2" s="8">
-        <v>33239</v>
+        <v>32115</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -558,7 +573,7 @@
         <v>21</v>
       </c>
       <c r="D3" s="8">
-        <v>33604</v>
+        <v>30423</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -572,7 +587,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="8">
-        <v>33970</v>
+        <v>30861</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -586,7 +601,7 @@
         <v>23</v>
       </c>
       <c r="D5" s="8">
-        <v>32874</v>
+        <v>29077</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -600,7 +615,7 @@
         <v>24</v>
       </c>
       <c r="D6" s="8">
-        <v>33239</v>
+        <v>29298</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -614,7 +629,7 @@
         <v>25</v>
       </c>
       <c r="D7" s="8">
-        <v>33970</v>
+        <v>29147</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -628,7 +643,7 @@
         <v>26</v>
       </c>
       <c r="D8" s="8">
-        <v>32509</v>
+        <v>27666</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -642,14 +657,22 @@
         <v>27</v>
       </c>
       <c r="D9" s="8">
-        <v>29587</v>
+        <v>29913</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="9"/>
+      <c r="A10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="9">
+        <v>25642</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>

</xml_diff>